<commit_message>
update the test cases for registration,search,vaccine administer,statistic
</commit_message>
<xml_diff>
--- a/vaccination.xlsx
+++ b/vaccination.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\VaccinationSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD05F1E-8FC6-4178-9BAC-29A5676DA098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81E5CC3-AA38-45C5-8789-100A8AE738A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{72EE0839-B996-4A20-9CBD-3540A773C11B}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="2" activeTab="2" xr2:uid="{72EE0839-B996-4A20-9CBD-3540A773C11B}"/>
   </bookViews>
   <sheets>
     <sheet name=" Patient Registration Module" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t xml:space="preserve"> Valid Scenarios</t>
   </si>
@@ -541,7 +541,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -670,79 +670,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEB2B56-0B0B-461B-8B9C-312C52727B3C}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -754,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35605D8E-B14B-4FA7-A853-D24D405F8A0F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,16 +797,25 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -806,10 +832,16 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>